<commit_message>
Variante mit i de Mitti ish jz no dezue cho und halt normal wenn 2 gsetzt sind das mer s dritte setzt.
</commit_message>
<xml_diff>
--- a/src/Dokumentation Teil 1/_210_Gantt-Diagramm.110.xlsx
+++ b/src/Dokumentation Teil 1/_210_Gantt-Diagramm.110.xlsx
@@ -9,7 +9,8 @@
   <sheets>
     <sheet name="Balkenplan" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -505,99 +506,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -614,12 +522,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -638,6 +540,105 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60 % - Akzent1" xfId="2" builtinId="32"/>
@@ -996,7 +997,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:85" s="2" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="23"/>
@@ -1007,109 +1008,109 @@
       <c r="E1" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="50">
+      <c r="F1" s="85">
         <v>5.0199999999999996</v>
       </c>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="50">
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="85">
         <v>6.02</v>
       </c>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="50">
+      <c r="O1" s="86"/>
+      <c r="P1" s="86"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
+      <c r="S1" s="86"/>
+      <c r="T1" s="86"/>
+      <c r="U1" s="87"/>
+      <c r="V1" s="85">
         <v>7.02</v>
       </c>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="52"/>
-      <c r="AD1" s="50">
+      <c r="W1" s="86"/>
+      <c r="X1" s="86"/>
+      <c r="Y1" s="86"/>
+      <c r="Z1" s="86"/>
+      <c r="AA1" s="86"/>
+      <c r="AB1" s="86"/>
+      <c r="AC1" s="87"/>
+      <c r="AD1" s="85">
         <v>8.02</v>
       </c>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="51"/>
-      <c r="AI1" s="51"/>
-      <c r="AJ1" s="51"/>
-      <c r="AK1" s="52"/>
-      <c r="AL1" s="50">
+      <c r="AE1" s="86"/>
+      <c r="AF1" s="86"/>
+      <c r="AG1" s="86"/>
+      <c r="AH1" s="86"/>
+      <c r="AI1" s="86"/>
+      <c r="AJ1" s="86"/>
+      <c r="AK1" s="87"/>
+      <c r="AL1" s="85">
         <v>9.02</v>
       </c>
-      <c r="AM1" s="51"/>
-      <c r="AN1" s="51"/>
-      <c r="AO1" s="51"/>
-      <c r="AP1" s="51"/>
-      <c r="AQ1" s="51"/>
-      <c r="AR1" s="51"/>
-      <c r="AS1" s="52"/>
-      <c r="AT1" s="50" t="s">
+      <c r="AM1" s="86"/>
+      <c r="AN1" s="86"/>
+      <c r="AO1" s="86"/>
+      <c r="AP1" s="86"/>
+      <c r="AQ1" s="86"/>
+      <c r="AR1" s="86"/>
+      <c r="AS1" s="87"/>
+      <c r="AT1" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="AU1" s="51"/>
-      <c r="AV1" s="51"/>
-      <c r="AW1" s="51"/>
-      <c r="AX1" s="51"/>
-      <c r="AY1" s="51"/>
-      <c r="AZ1" s="51"/>
-      <c r="BA1" s="52"/>
-      <c r="BB1" s="50">
+      <c r="AU1" s="86"/>
+      <c r="AV1" s="86"/>
+      <c r="AW1" s="86"/>
+      <c r="AX1" s="86"/>
+      <c r="AY1" s="86"/>
+      <c r="AZ1" s="86"/>
+      <c r="BA1" s="87"/>
+      <c r="BB1" s="85">
         <v>19.02</v>
       </c>
-      <c r="BC1" s="51"/>
-      <c r="BD1" s="51"/>
-      <c r="BE1" s="51"/>
-      <c r="BF1" s="51"/>
-      <c r="BG1" s="51"/>
-      <c r="BH1" s="51"/>
-      <c r="BI1" s="52"/>
-      <c r="BJ1" s="50">
+      <c r="BC1" s="86"/>
+      <c r="BD1" s="86"/>
+      <c r="BE1" s="86"/>
+      <c r="BF1" s="86"/>
+      <c r="BG1" s="86"/>
+      <c r="BH1" s="86"/>
+      <c r="BI1" s="87"/>
+      <c r="BJ1" s="85">
         <v>20.02</v>
       </c>
-      <c r="BK1" s="51"/>
-      <c r="BL1" s="51"/>
-      <c r="BM1" s="51"/>
-      <c r="BN1" s="51"/>
-      <c r="BO1" s="51"/>
-      <c r="BP1" s="51"/>
-      <c r="BQ1" s="52"/>
-      <c r="BR1" s="50">
+      <c r="BK1" s="86"/>
+      <c r="BL1" s="86"/>
+      <c r="BM1" s="86"/>
+      <c r="BN1" s="86"/>
+      <c r="BO1" s="86"/>
+      <c r="BP1" s="86"/>
+      <c r="BQ1" s="87"/>
+      <c r="BR1" s="85">
         <v>21.02</v>
       </c>
-      <c r="BS1" s="51"/>
-      <c r="BT1" s="51"/>
-      <c r="BU1" s="51"/>
-      <c r="BV1" s="51"/>
-      <c r="BW1" s="51"/>
-      <c r="BX1" s="51"/>
-      <c r="BY1" s="52"/>
-      <c r="BZ1" s="50">
+      <c r="BS1" s="86"/>
+      <c r="BT1" s="86"/>
+      <c r="BU1" s="86"/>
+      <c r="BV1" s="86"/>
+      <c r="BW1" s="86"/>
+      <c r="BX1" s="86"/>
+      <c r="BY1" s="87"/>
+      <c r="BZ1" s="85">
         <v>22.02</v>
       </c>
-      <c r="CA1" s="51"/>
-      <c r="CB1" s="51"/>
-      <c r="CC1" s="51"/>
-      <c r="CD1" s="51"/>
-      <c r="CE1" s="51"/>
-      <c r="CF1" s="51"/>
-      <c r="CG1" s="52"/>
+      <c r="CA1" s="86"/>
+      <c r="CB1" s="86"/>
+      <c r="CC1" s="86"/>
+      <c r="CD1" s="86"/>
+      <c r="CE1" s="86"/>
+      <c r="CF1" s="86"/>
+      <c r="CG1" s="87"/>
     </row>
     <row r="2" spans="1:85" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="66"/>
+      <c r="A2" s="84"/>
       <c r="B2" s="22" t="s">
         <v>12</v>
       </c>
@@ -1362,25 +1363,25 @@
       </c>
     </row>
     <row r="3" spans="1:85" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="56">
+      <c r="A3" s="82">
         <v>1</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="67" t="s">
+      <c r="C3" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="67"/>
+      <c r="D3" s="92"/>
       <c r="E3" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="79"/>
-      <c r="G3" s="80"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="95"/>
       <c r="M3" s="11"/>
-      <c r="N3" s="94"/>
-      <c r="O3" s="95"/>
-      <c r="P3" s="95"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="62"/>
+      <c r="P3" s="62"/>
       <c r="U3" s="11"/>
       <c r="V3" s="9"/>
       <c r="AC3" s="11"/>
@@ -1400,10 +1401,10 @@
       <c r="CG3" s="11"/>
     </row>
     <row r="4" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
+      <c r="A4" s="82"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
       <c r="E4" s="39" t="s">
         <v>28</v>
       </c>
@@ -1419,19 +1420,19 @@
       <c r="CG4" s="13"/>
     </row>
     <row r="5" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="56"/>
-      <c r="B5" s="64"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
+      <c r="A5" s="82"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
       <c r="E5" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
       <c r="M5" s="13"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
       <c r="U5" s="13"/>
       <c r="AC5" s="13"/>
       <c r="AK5" s="13"/>
@@ -1443,10 +1444,10 @@
       <c r="CG5" s="13"/>
     </row>
     <row r="6" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="56"/>
-      <c r="B6" s="64"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
+      <c r="A6" s="82"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="93"/>
+      <c r="D6" s="93"/>
       <c r="E6" s="39" t="s">
         <v>34</v>
       </c>
@@ -1535,21 +1536,21 @@
       <c r="A7" s="48"/>
       <c r="B7" s="47"/>
       <c r="C7" s="49"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="85" t="s">
+      <c r="D7" s="52"/>
+      <c r="E7" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="81"/>
-      <c r="G7" s="81"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
       <c r="M7" s="13"/>
-      <c r="N7" s="81"/>
-      <c r="O7" s="81"/>
-      <c r="P7" s="81"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
       <c r="Q7" s="12"/>
       <c r="R7" s="12"/>
       <c r="S7" s="12"/>
@@ -1624,8 +1625,8 @@
       <c r="A8" s="48"/>
       <c r="B8" s="47"/>
       <c r="C8" s="49"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="82" t="s">
+      <c r="D8" s="53"/>
+      <c r="E8" s="51" t="s">
         <v>32</v>
       </c>
       <c r="F8" s="12"/>
@@ -1710,16 +1711,16 @@
       <c r="CG8" s="13"/>
     </row>
     <row r="9" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="56">
+      <c r="A9" s="82">
         <v>2</v>
       </c>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="75" t="s">
+      <c r="C9" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="76"/>
+      <c r="D9" s="89"/>
       <c r="E9" s="25" t="s">
         <v>27</v>
       </c>
@@ -1727,9 +1728,9 @@
       <c r="M9" s="17"/>
       <c r="N9" s="15"/>
       <c r="U9" s="17"/>
-      <c r="V9" s="94"/>
-      <c r="W9" s="95"/>
-      <c r="X9" s="95"/>
+      <c r="V9" s="61"/>
+      <c r="W9" s="62"/>
+      <c r="X9" s="62"/>
       <c r="AC9" s="17"/>
       <c r="AD9" s="15"/>
       <c r="AK9" s="17"/>
@@ -1747,10 +1748,10 @@
       <c r="CG9" s="17"/>
     </row>
     <row r="10" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
-      <c r="B10" s="58"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="78"/>
+      <c r="A10" s="82"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="91"/>
       <c r="E10" s="41" t="s">
         <v>28</v>
       </c>
@@ -1776,10 +1777,10 @@
       <c r="CG10" s="20"/>
     </row>
     <row r="11" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="56"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="78"/>
+      <c r="A11" s="82"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="91"/>
       <c r="E11" s="26" t="s">
         <v>33</v>
       </c>
@@ -1787,9 +1788,9 @@
       <c r="M11" s="20"/>
       <c r="N11" s="18"/>
       <c r="U11" s="20"/>
-      <c r="V11" s="96"/>
-      <c r="W11" s="81"/>
-      <c r="X11" s="81"/>
+      <c r="V11" s="63"/>
+      <c r="W11" s="50"/>
+      <c r="X11" s="50"/>
       <c r="AC11" s="20"/>
       <c r="AD11" s="18"/>
       <c r="AK11" s="20"/>
@@ -1807,10 +1808,10 @@
       <c r="CG11" s="20"/>
     </row>
     <row r="12" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
+      <c r="A12" s="82"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
       <c r="E12" s="41" t="s">
         <v>34</v>
       </c>
@@ -1898,8 +1899,8 @@
     <row r="13" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="48"/>
       <c r="B13" s="45"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
       <c r="E13" s="41" t="s">
         <v>31</v>
       </c>
@@ -1919,9 +1920,9 @@
       <c r="S13" s="19"/>
       <c r="T13" s="19"/>
       <c r="U13" s="20"/>
-      <c r="V13" s="96"/>
-      <c r="W13" s="81"/>
-      <c r="X13" s="81"/>
+      <c r="V13" s="63"/>
+      <c r="W13" s="50"/>
+      <c r="X13" s="50"/>
       <c r="Y13" s="19"/>
       <c r="Z13" s="19"/>
       <c r="AA13" s="19"/>
@@ -1987,8 +1988,8 @@
     <row r="14" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="48"/>
       <c r="B14" s="45"/>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
       <c r="E14" s="41" t="s">
         <v>32</v>
       </c>
@@ -2074,17 +2075,17 @@
       <c r="CG14" s="20"/>
     </row>
     <row r="15" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="56">
+      <c r="A15" s="82">
         <v>3</v>
       </c>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="67"/>
-      <c r="E15" s="93" t="s">
+      <c r="D15" s="92"/>
+      <c r="E15" s="60" t="s">
         <v>27</v>
       </c>
       <c r="F15" s="9"/>
@@ -2092,11 +2093,11 @@
       <c r="N15" s="9"/>
       <c r="U15" s="11"/>
       <c r="V15" s="9"/>
-      <c r="Y15" s="95"/>
-      <c r="Z15" s="95"/>
-      <c r="AA15" s="95"/>
-      <c r="AB15" s="95"/>
-      <c r="AC15" s="97"/>
+      <c r="Y15" s="62"/>
+      <c r="Z15" s="62"/>
+      <c r="AA15" s="62"/>
+      <c r="AB15" s="62"/>
+      <c r="AC15" s="64"/>
       <c r="AD15" s="9"/>
       <c r="AK15" s="11"/>
       <c r="AL15" s="9"/>
@@ -2113,10 +2114,10 @@
       <c r="CG15" s="11"/>
     </row>
     <row r="16" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="56"/>
-      <c r="B16" s="64"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="89"/>
+      <c r="A16" s="82"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="96"/>
       <c r="E16" s="39" t="s">
         <v>28</v>
       </c>
@@ -2132,20 +2133,20 @@
       <c r="CG16" s="13"/>
     </row>
     <row r="17" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="56"/>
-      <c r="B17" s="64"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="89"/>
+      <c r="A17" s="82"/>
+      <c r="B17" s="80"/>
+      <c r="C17" s="93"/>
+      <c r="D17" s="96"/>
       <c r="E17" s="40" t="s">
         <v>33</v>
       </c>
       <c r="M17" s="13"/>
       <c r="U17" s="13"/>
-      <c r="Y17" s="81"/>
-      <c r="Z17" s="81"/>
-      <c r="AA17" s="81"/>
-      <c r="AB17" s="81"/>
-      <c r="AC17" s="98"/>
+      <c r="Y17" s="50"/>
+      <c r="Z17" s="50"/>
+      <c r="AA17" s="50"/>
+      <c r="AB17" s="50"/>
+      <c r="AC17" s="65"/>
       <c r="AK17" s="13"/>
       <c r="AS17" s="13"/>
       <c r="BA17" s="13"/>
@@ -2155,10 +2156,10 @@
       <c r="CG17" s="13"/>
     </row>
     <row r="18" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="56"/>
-      <c r="B18" s="64"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="89"/>
+      <c r="A18" s="82"/>
+      <c r="B18" s="80"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="96"/>
       <c r="E18" s="39" t="s">
         <v>34</v>
       </c>
@@ -2248,7 +2249,7 @@
       <c r="B19" s="47"/>
       <c r="C19" s="49"/>
       <c r="D19" s="49"/>
-      <c r="E19" s="90" t="s">
+      <c r="E19" s="57" t="s">
         <v>31</v>
       </c>
       <c r="F19" s="12"/>
@@ -2270,11 +2271,11 @@
       <c r="V19" s="12"/>
       <c r="W19" s="12"/>
       <c r="X19" s="12"/>
-      <c r="Y19" s="81"/>
-      <c r="Z19" s="81"/>
-      <c r="AA19" s="81"/>
-      <c r="AB19" s="81"/>
-      <c r="AC19" s="98"/>
+      <c r="Y19" s="50"/>
+      <c r="Z19" s="50"/>
+      <c r="AA19" s="50"/>
+      <c r="AB19" s="50"/>
+      <c r="AC19" s="65"/>
       <c r="AD19" s="12"/>
       <c r="AE19" s="12"/>
       <c r="AF19" s="12"/>
@@ -2337,7 +2338,7 @@
       <c r="B20" s="47"/>
       <c r="C20" s="49"/>
       <c r="D20" s="49"/>
-      <c r="E20" s="90" t="s">
+      <c r="E20" s="57" t="s">
         <v>32</v>
       </c>
       <c r="F20" s="12"/>
@@ -2422,16 +2423,16 @@
       <c r="CG20" s="13"/>
     </row>
     <row r="21" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="56">
+      <c r="A21" s="82">
         <v>4</v>
       </c>
-      <c r="B21" s="61" t="s">
+      <c r="B21" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="75" t="s">
+      <c r="C21" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="76"/>
+      <c r="D21" s="89"/>
       <c r="E21" s="25" t="s">
         <v>27</v>
       </c>
@@ -2445,14 +2446,14 @@
       <c r="AK21" s="17"/>
       <c r="AL21" s="15"/>
       <c r="AS21" s="17"/>
-      <c r="AT21" s="94"/>
-      <c r="AU21" s="95"/>
-      <c r="AV21" s="95"/>
-      <c r="AW21" s="95"/>
-      <c r="AX21" s="95"/>
-      <c r="AY21" s="95"/>
-      <c r="AZ21" s="95"/>
-      <c r="BA21" s="97"/>
+      <c r="AT21" s="61"/>
+      <c r="AU21" s="62"/>
+      <c r="AV21" s="62"/>
+      <c r="AW21" s="62"/>
+      <c r="AX21" s="62"/>
+      <c r="AY21" s="62"/>
+      <c r="AZ21" s="62"/>
+      <c r="BA21" s="64"/>
       <c r="BB21" s="15"/>
       <c r="BI21" s="17"/>
       <c r="BJ21" s="15"/>
@@ -2463,10 +2464,10 @@
       <c r="CG21" s="17"/>
     </row>
     <row r="22" spans="1:85" s="19" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="56"/>
-      <c r="B22" s="58"/>
-      <c r="C22" s="77"/>
-      <c r="D22" s="78"/>
+      <c r="A22" s="82"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="90"/>
+      <c r="D22" s="91"/>
       <c r="E22" s="41" t="s">
         <v>29</v>
       </c>
@@ -2492,10 +2493,10 @@
       <c r="CG22" s="20"/>
     </row>
     <row r="23" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="56"/>
-      <c r="B23" s="58"/>
-      <c r="C23" s="77"/>
-      <c r="D23" s="78"/>
+      <c r="A23" s="82"/>
+      <c r="B23" s="70"/>
+      <c r="C23" s="90"/>
+      <c r="D23" s="91"/>
       <c r="E23" s="26" t="s">
         <v>33</v>
       </c>
@@ -2511,32 +2512,32 @@
       <c r="AS23" s="20"/>
       <c r="AT23" s="18"/>
       <c r="BA23" s="20"/>
-      <c r="BB23" s="96"/>
-      <c r="BC23" s="81"/>
-      <c r="BD23" s="81"/>
-      <c r="BE23" s="81"/>
-      <c r="BF23" s="81"/>
-      <c r="BG23" s="81"/>
-      <c r="BH23" s="81"/>
-      <c r="BI23" s="98"/>
-      <c r="BJ23" s="96"/>
-      <c r="BK23" s="81"/>
-      <c r="BL23" s="81"/>
-      <c r="BM23" s="81"/>
-      <c r="BN23" s="81"/>
-      <c r="BO23" s="81"/>
-      <c r="BP23" s="81"/>
-      <c r="BQ23" s="98"/>
+      <c r="BB23" s="63"/>
+      <c r="BC23" s="50"/>
+      <c r="BD23" s="50"/>
+      <c r="BE23" s="50"/>
+      <c r="BF23" s="50"/>
+      <c r="BG23" s="50"/>
+      <c r="BH23" s="50"/>
+      <c r="BI23" s="65"/>
+      <c r="BJ23" s="63"/>
+      <c r="BK23" s="50"/>
+      <c r="BL23" s="50"/>
+      <c r="BM23" s="50"/>
+      <c r="BN23" s="50"/>
+      <c r="BO23" s="50"/>
+      <c r="BP23" s="50"/>
+      <c r="BQ23" s="65"/>
       <c r="BR23" s="18"/>
       <c r="BY23" s="20"/>
       <c r="BZ23" s="18"/>
       <c r="CG23" s="20"/>
     </row>
     <row r="24" spans="1:85" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="56"/>
-      <c r="B24" s="58"/>
-      <c r="C24" s="78"/>
-      <c r="D24" s="78"/>
+      <c r="A24" s="82"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="91"/>
+      <c r="D24" s="91"/>
       <c r="E24" s="41" t="s">
         <v>34</v>
       </c>
@@ -2624,9 +2625,9 @@
     <row r="25" spans="1:85" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="48"/>
       <c r="B25" s="45"/>
-      <c r="C25" s="86"/>
-      <c r="D25" s="91"/>
-      <c r="E25" s="87" t="s">
+      <c r="C25" s="55"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="56" t="s">
         <v>31</v>
       </c>
       <c r="F25" s="18"/>
@@ -2677,22 +2678,22 @@
       <c r="AY25" s="19"/>
       <c r="AZ25" s="19"/>
       <c r="BA25" s="20"/>
-      <c r="BB25" s="96"/>
-      <c r="BC25" s="81"/>
-      <c r="BD25" s="81"/>
-      <c r="BE25" s="81"/>
-      <c r="BF25" s="81"/>
-      <c r="BG25" s="81"/>
-      <c r="BH25" s="81"/>
-      <c r="BI25" s="98"/>
-      <c r="BJ25" s="96"/>
-      <c r="BK25" s="81"/>
-      <c r="BL25" s="81"/>
-      <c r="BM25" s="81"/>
-      <c r="BN25" s="81"/>
-      <c r="BO25" s="81"/>
-      <c r="BP25" s="81"/>
-      <c r="BQ25" s="98"/>
+      <c r="BB25" s="63"/>
+      <c r="BC25" s="50"/>
+      <c r="BD25" s="50"/>
+      <c r="BE25" s="50"/>
+      <c r="BF25" s="50"/>
+      <c r="BG25" s="50"/>
+      <c r="BH25" s="50"/>
+      <c r="BI25" s="65"/>
+      <c r="BJ25" s="63"/>
+      <c r="BK25" s="50"/>
+      <c r="BL25" s="50"/>
+      <c r="BM25" s="50"/>
+      <c r="BN25" s="50"/>
+      <c r="BO25" s="50"/>
+      <c r="BP25" s="50"/>
+      <c r="BQ25" s="65"/>
       <c r="BR25" s="18"/>
       <c r="BS25" s="19"/>
       <c r="BT25" s="19"/>
@@ -2713,9 +2714,9 @@
     <row r="26" spans="1:85" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="48"/>
       <c r="B26" s="45"/>
-      <c r="C26" s="86"/>
-      <c r="D26" s="92"/>
-      <c r="E26" s="87" t="s">
+      <c r="C26" s="55"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="56" t="s">
         <v>32</v>
       </c>
       <c r="F26" s="18"/>
@@ -2800,16 +2801,16 @@
       <c r="CG26" s="20"/>
     </row>
     <row r="27" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="56">
+      <c r="A27" s="82">
         <v>5</v>
       </c>
-      <c r="B27" s="53" t="s">
+      <c r="B27" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="67" t="s">
+      <c r="C27" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="88"/>
+      <c r="D27" s="97"/>
       <c r="E27" s="38" t="s">
         <v>27</v>
       </c>
@@ -2835,10 +2836,10 @@
       <c r="CG27" s="11"/>
     </row>
     <row r="28" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="56"/>
-      <c r="B28" s="64"/>
-      <c r="C28" s="68"/>
-      <c r="D28" s="89"/>
+      <c r="A28" s="82"/>
+      <c r="B28" s="80"/>
+      <c r="C28" s="93"/>
+      <c r="D28" s="96"/>
       <c r="E28" s="39" t="s">
         <v>28</v>
       </c>
@@ -2854,10 +2855,10 @@
       <c r="CG28" s="13"/>
     </row>
     <row r="29" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="56"/>
-      <c r="B29" s="64"/>
-      <c r="C29" s="68"/>
-      <c r="D29" s="89"/>
+      <c r="A29" s="82"/>
+      <c r="B29" s="80"/>
+      <c r="C29" s="93"/>
+      <c r="D29" s="96"/>
       <c r="E29" s="40" t="s">
         <v>33</v>
       </c>
@@ -2867,19 +2868,19 @@
       <c r="AK29" s="13"/>
       <c r="AS29" s="13"/>
       <c r="BA29" s="13"/>
-      <c r="BB29" s="81"/>
-      <c r="BC29" s="81"/>
-      <c r="BD29" s="81"/>
+      <c r="BB29" s="50"/>
+      <c r="BC29" s="50"/>
+      <c r="BD29" s="50"/>
       <c r="BI29" s="13"/>
       <c r="BQ29" s="13"/>
       <c r="BY29" s="13"/>
       <c r="CG29" s="13"/>
     </row>
     <row r="30" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="56"/>
-      <c r="B30" s="64"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="89"/>
+      <c r="A30" s="82"/>
+      <c r="B30" s="80"/>
+      <c r="C30" s="93"/>
+      <c r="D30" s="96"/>
       <c r="E30" s="39" t="s">
         <v>34</v>
       </c>
@@ -2968,8 +2969,8 @@
       <c r="A31" s="48"/>
       <c r="B31" s="47"/>
       <c r="C31" s="49"/>
-      <c r="D31" s="83"/>
-      <c r="E31" s="82" t="s">
+      <c r="D31" s="52"/>
+      <c r="E31" s="51" t="s">
         <v>31</v>
       </c>
       <c r="F31" s="12"/>
@@ -3057,8 +3058,8 @@
       <c r="A32" s="48"/>
       <c r="B32" s="47"/>
       <c r="C32" s="49"/>
-      <c r="D32" s="84"/>
-      <c r="E32" s="82" t="s">
+      <c r="D32" s="53"/>
+      <c r="E32" s="51" t="s">
         <v>32</v>
       </c>
       <c r="F32" s="12"/>
@@ -3143,16 +3144,16 @@
       <c r="CG32" s="13"/>
     </row>
     <row r="33" spans="1:85" s="16" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="56">
+      <c r="A33" s="82">
         <v>6</v>
       </c>
-      <c r="B33" s="61" t="s">
+      <c r="B33" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="75" t="s">
+      <c r="C33" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="76"/>
+      <c r="D33" s="89"/>
       <c r="E33" s="25" t="s">
         <v>27</v>
       </c>
@@ -3178,10 +3179,10 @@
       <c r="CG33" s="17"/>
     </row>
     <row r="34" spans="1:85" s="19" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="56"/>
-      <c r="B34" s="58"/>
-      <c r="C34" s="77"/>
-      <c r="D34" s="78"/>
+      <c r="A34" s="82"/>
+      <c r="B34" s="70"/>
+      <c r="C34" s="90"/>
+      <c r="D34" s="91"/>
       <c r="E34" s="41" t="s">
         <v>29</v>
       </c>
@@ -3207,10 +3208,10 @@
       <c r="CG34" s="20"/>
     </row>
     <row r="35" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="56"/>
-      <c r="B35" s="58"/>
-      <c r="C35" s="77"/>
-      <c r="D35" s="78"/>
+      <c r="A35" s="82"/>
+      <c r="B35" s="70"/>
+      <c r="C35" s="90"/>
+      <c r="D35" s="91"/>
       <c r="E35" s="26" t="s">
         <v>33</v>
       </c>
@@ -3236,10 +3237,10 @@
       <c r="CG35" s="20"/>
     </row>
     <row r="36" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="56"/>
-      <c r="B36" s="58"/>
-      <c r="C36" s="78"/>
-      <c r="D36" s="78"/>
+      <c r="A36" s="82"/>
+      <c r="B36" s="70"/>
+      <c r="C36" s="91"/>
+      <c r="D36" s="91"/>
       <c r="E36" s="41" t="s">
         <v>34</v>
       </c>
@@ -3327,8 +3328,8 @@
     <row r="37" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="48"/>
       <c r="B37" s="45"/>
-      <c r="C37" s="86"/>
-      <c r="D37" s="86"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
       <c r="E37" s="41" t="s">
         <v>31</v>
       </c>
@@ -3356,7 +3357,7 @@
       <c r="AA37" s="19"/>
       <c r="AB37" s="19"/>
       <c r="AC37" s="20"/>
-      <c r="AD37" s="96"/>
+      <c r="AD37" s="63"/>
       <c r="AE37" s="19"/>
       <c r="AF37" s="19"/>
       <c r="AG37" s="19"/>
@@ -3416,8 +3417,8 @@
     <row r="38" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="48"/>
       <c r="B38" s="45"/>
-      <c r="C38" s="86"/>
-      <c r="D38" s="86"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="55"/>
       <c r="E38" s="41" t="s">
         <v>32</v>
       </c>
@@ -3503,17 +3504,17 @@
       <c r="CG38" s="20"/>
     </row>
     <row r="39" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="56">
+      <c r="A39" s="82">
         <v>7</v>
       </c>
-      <c r="B39" s="53" t="s">
+      <c r="B39" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="67" t="s">
+      <c r="C39" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="D39" s="67"/>
-      <c r="E39" s="93" t="s">
+      <c r="D39" s="92"/>
+      <c r="E39" s="60" t="s">
         <v>27</v>
       </c>
       <c r="F39" s="9"/>
@@ -3538,10 +3539,10 @@
       <c r="CG39" s="11"/>
     </row>
     <row r="40" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="56"/>
-      <c r="B40" s="54"/>
-      <c r="C40" s="68"/>
-      <c r="D40" s="89"/>
+      <c r="A40" s="82"/>
+      <c r="B40" s="67"/>
+      <c r="C40" s="93"/>
+      <c r="D40" s="96"/>
       <c r="E40" s="39" t="s">
         <v>30</v>
       </c>
@@ -3557,16 +3558,16 @@
       <c r="CG40" s="13"/>
     </row>
     <row r="41" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="56"/>
-      <c r="B41" s="54"/>
-      <c r="C41" s="68"/>
-      <c r="D41" s="89"/>
+      <c r="A41" s="82"/>
+      <c r="B41" s="67"/>
+      <c r="C41" s="93"/>
+      <c r="D41" s="96"/>
       <c r="E41" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="H41" s="81"/>
+      <c r="H41" s="50"/>
       <c r="M41" s="13"/>
-      <c r="Q41" s="81"/>
+      <c r="Q41" s="50"/>
       <c r="U41" s="13"/>
       <c r="AC41" s="13"/>
       <c r="AK41" s="13"/>
@@ -3578,10 +3579,10 @@
       <c r="CG41" s="13"/>
     </row>
     <row r="42" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="56"/>
-      <c r="B42" s="54"/>
-      <c r="C42" s="68"/>
-      <c r="D42" s="89"/>
+      <c r="A42" s="82"/>
+      <c r="B42" s="67"/>
+      <c r="C42" s="93"/>
+      <c r="D42" s="96"/>
       <c r="E42" s="39" t="s">
         <v>34</v>
       </c>
@@ -3671,7 +3672,7 @@
       <c r="B43" s="44"/>
       <c r="C43" s="49"/>
       <c r="D43" s="49"/>
-      <c r="E43" s="90" t="s">
+      <c r="E43" s="57" t="s">
         <v>31</v>
       </c>
       <c r="F43" s="12"/>
@@ -3760,7 +3761,7 @@
       <c r="B44" s="44"/>
       <c r="C44" s="49"/>
       <c r="D44" s="49"/>
-      <c r="E44" s="90" t="s">
+      <c r="E44" s="57" t="s">
         <v>32</v>
       </c>
       <c r="F44" s="12"/>
@@ -3845,16 +3846,16 @@
       <c r="CG44" s="13"/>
     </row>
     <row r="45" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="56">
+      <c r="A45" s="82">
         <v>8</v>
       </c>
-      <c r="B45" s="61" t="s">
+      <c r="B45" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="75" t="s">
+      <c r="C45" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="D45" s="76"/>
+      <c r="D45" s="89"/>
       <c r="E45" s="25" t="s">
         <v>27</v>
       </c>
@@ -3880,10 +3881,10 @@
       <c r="CG45" s="17"/>
     </row>
     <row r="46" spans="1:85" s="19" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="56"/>
-      <c r="B46" s="63"/>
-      <c r="C46" s="77"/>
-      <c r="D46" s="78"/>
+      <c r="A46" s="82"/>
+      <c r="B46" s="78"/>
+      <c r="C46" s="90"/>
+      <c r="D46" s="91"/>
       <c r="E46" s="41" t="s">
         <v>29</v>
       </c>
@@ -3909,10 +3910,10 @@
       <c r="CG46" s="20"/>
     </row>
     <row r="47" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="56"/>
-      <c r="B47" s="63"/>
-      <c r="C47" s="77"/>
-      <c r="D47" s="78"/>
+      <c r="A47" s="82"/>
+      <c r="B47" s="78"/>
+      <c r="C47" s="90"/>
+      <c r="D47" s="91"/>
       <c r="E47" s="26" t="s">
         <v>33</v>
       </c>
@@ -3928,44 +3929,44 @@
       <c r="AS47" s="20"/>
       <c r="AT47" s="18"/>
       <c r="BA47" s="20"/>
-      <c r="BB47" s="96"/>
-      <c r="BC47" s="81"/>
-      <c r="BD47" s="81"/>
-      <c r="BE47" s="81"/>
-      <c r="BF47" s="81"/>
-      <c r="BG47" s="81"/>
-      <c r="BH47" s="81"/>
-      <c r="BI47" s="98"/>
-      <c r="BJ47" s="96"/>
-      <c r="BK47" s="81"/>
-      <c r="BL47" s="81"/>
-      <c r="BM47" s="81"/>
-      <c r="BN47" s="81"/>
-      <c r="BO47" s="81"/>
-      <c r="BP47" s="81"/>
-      <c r="BQ47" s="98"/>
-      <c r="BR47" s="96"/>
-      <c r="BS47" s="81"/>
-      <c r="BT47" s="81"/>
-      <c r="BU47" s="81"/>
-      <c r="BV47" s="81"/>
-      <c r="BW47" s="81"/>
-      <c r="BX47" s="81"/>
-      <c r="BY47" s="98"/>
-      <c r="BZ47" s="96"/>
-      <c r="CA47" s="81"/>
-      <c r="CB47" s="81"/>
-      <c r="CC47" s="81"/>
-      <c r="CD47" s="81"/>
-      <c r="CE47" s="81"/>
-      <c r="CF47" s="81"/>
-      <c r="CG47" s="98"/>
+      <c r="BB47" s="63"/>
+      <c r="BC47" s="50"/>
+      <c r="BD47" s="50"/>
+      <c r="BE47" s="50"/>
+      <c r="BF47" s="50"/>
+      <c r="BG47" s="50"/>
+      <c r="BH47" s="50"/>
+      <c r="BI47" s="65"/>
+      <c r="BJ47" s="63"/>
+      <c r="BK47" s="50"/>
+      <c r="BL47" s="50"/>
+      <c r="BM47" s="50"/>
+      <c r="BN47" s="50"/>
+      <c r="BO47" s="50"/>
+      <c r="BP47" s="50"/>
+      <c r="BQ47" s="65"/>
+      <c r="BR47" s="63"/>
+      <c r="BS47" s="50"/>
+      <c r="BT47" s="50"/>
+      <c r="BU47" s="50"/>
+      <c r="BV47" s="50"/>
+      <c r="BW47" s="50"/>
+      <c r="BX47" s="50"/>
+      <c r="BY47" s="65"/>
+      <c r="BZ47" s="63"/>
+      <c r="CA47" s="50"/>
+      <c r="CB47" s="50"/>
+      <c r="CC47" s="50"/>
+      <c r="CD47" s="50"/>
+      <c r="CE47" s="50"/>
+      <c r="CF47" s="50"/>
+      <c r="CG47" s="65"/>
     </row>
     <row r="48" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="56"/>
-      <c r="B48" s="63"/>
-      <c r="C48" s="78"/>
-      <c r="D48" s="78"/>
+      <c r="A48" s="82"/>
+      <c r="B48" s="78"/>
+      <c r="C48" s="91"/>
+      <c r="D48" s="91"/>
       <c r="E48" s="41" t="s">
         <v>34</v>
       </c>
@@ -4053,8 +4054,8 @@
     <row r="49" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="48"/>
       <c r="B49" s="46"/>
-      <c r="C49" s="86"/>
-      <c r="D49" s="86"/>
+      <c r="C49" s="55"/>
+      <c r="D49" s="55"/>
       <c r="E49" s="41" t="s">
         <v>31</v>
       </c>
@@ -4106,30 +4107,30 @@
       <c r="AY49" s="19"/>
       <c r="AZ49" s="19"/>
       <c r="BA49" s="20"/>
-      <c r="BB49" s="96"/>
-      <c r="BC49" s="81"/>
-      <c r="BD49" s="81"/>
-      <c r="BE49" s="81"/>
-      <c r="BF49" s="81"/>
-      <c r="BG49" s="81"/>
-      <c r="BH49" s="81"/>
-      <c r="BI49" s="98"/>
-      <c r="BJ49" s="96"/>
-      <c r="BK49" s="81"/>
-      <c r="BL49" s="81"/>
-      <c r="BM49" s="81"/>
-      <c r="BN49" s="81"/>
-      <c r="BO49" s="81"/>
-      <c r="BP49" s="81"/>
-      <c r="BQ49" s="98"/>
-      <c r="BR49" s="96"/>
-      <c r="BS49" s="81"/>
-      <c r="BT49" s="81"/>
-      <c r="BU49" s="81"/>
-      <c r="BV49" s="81"/>
-      <c r="BW49" s="81"/>
-      <c r="BX49" s="81"/>
-      <c r="BY49" s="98"/>
+      <c r="BB49" s="63"/>
+      <c r="BC49" s="50"/>
+      <c r="BD49" s="50"/>
+      <c r="BE49" s="50"/>
+      <c r="BF49" s="50"/>
+      <c r="BG49" s="50"/>
+      <c r="BH49" s="50"/>
+      <c r="BI49" s="65"/>
+      <c r="BJ49" s="63"/>
+      <c r="BK49" s="50"/>
+      <c r="BL49" s="50"/>
+      <c r="BM49" s="50"/>
+      <c r="BN49" s="50"/>
+      <c r="BO49" s="50"/>
+      <c r="BP49" s="50"/>
+      <c r="BQ49" s="65"/>
+      <c r="BR49" s="63"/>
+      <c r="BS49" s="50"/>
+      <c r="BT49" s="50"/>
+      <c r="BU49" s="50"/>
+      <c r="BV49" s="50"/>
+      <c r="BW49" s="50"/>
+      <c r="BX49" s="50"/>
+      <c r="BY49" s="65"/>
       <c r="BZ49" s="18"/>
       <c r="CA49" s="19"/>
       <c r="CB49" s="19"/>
@@ -4142,8 +4143,8 @@
     <row r="50" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="48"/>
       <c r="B50" s="46"/>
-      <c r="C50" s="86"/>
-      <c r="D50" s="86"/>
+      <c r="C50" s="55"/>
+      <c r="D50" s="55"/>
       <c r="E50" s="41" t="s">
         <v>32</v>
       </c>
@@ -4229,17 +4230,17 @@
       <c r="CG50" s="20"/>
     </row>
     <row r="51" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="56">
+      <c r="A51" s="82">
         <v>9</v>
       </c>
-      <c r="B51" s="53" t="s">
+      <c r="B51" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="C51" s="67" t="s">
+      <c r="C51" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="D51" s="67"/>
-      <c r="E51" s="93" t="s">
+      <c r="D51" s="92"/>
+      <c r="E51" s="60" t="s">
         <v>27</v>
       </c>
       <c r="F51" s="9"/>
@@ -4264,10 +4265,10 @@
       <c r="CG51" s="11"/>
     </row>
     <row r="52" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="56"/>
-      <c r="B52" s="54"/>
-      <c r="C52" s="68"/>
-      <c r="D52" s="89"/>
+      <c r="A52" s="82"/>
+      <c r="B52" s="67"/>
+      <c r="C52" s="93"/>
+      <c r="D52" s="96"/>
       <c r="E52" s="39" t="s">
         <v>28</v>
       </c>
@@ -4283,10 +4284,10 @@
       <c r="CG52" s="13"/>
     </row>
     <row r="53" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="56"/>
-      <c r="B53" s="54"/>
-      <c r="C53" s="68"/>
-      <c r="D53" s="89"/>
+      <c r="A53" s="82"/>
+      <c r="B53" s="67"/>
+      <c r="C53" s="93"/>
+      <c r="D53" s="96"/>
       <c r="E53" s="40" t="s">
         <v>33</v>
       </c>
@@ -4302,10 +4303,10 @@
       <c r="CG53" s="13"/>
     </row>
     <row r="54" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="56"/>
-      <c r="B54" s="54"/>
-      <c r="C54" s="68"/>
-      <c r="D54" s="89"/>
+      <c r="A54" s="82"/>
+      <c r="B54" s="67"/>
+      <c r="C54" s="93"/>
+      <c r="D54" s="96"/>
       <c r="E54" s="39" t="s">
         <v>34</v>
       </c>
@@ -4394,8 +4395,8 @@
       <c r="A55" s="48"/>
       <c r="B55" s="44"/>
       <c r="C55" s="49"/>
-      <c r="D55" s="83"/>
-      <c r="E55" s="82" t="s">
+      <c r="D55" s="52"/>
+      <c r="E55" s="51" t="s">
         <v>31</v>
       </c>
       <c r="F55" s="12"/>
@@ -4424,14 +4425,14 @@
       <c r="AC55" s="13"/>
       <c r="AD55" s="12"/>
       <c r="AE55" s="12"/>
-      <c r="AF55" s="81"/>
+      <c r="AF55" s="50"/>
       <c r="AG55" s="12"/>
       <c r="AH55" s="12"/>
       <c r="AI55" s="12"/>
       <c r="AJ55" s="12"/>
       <c r="AK55" s="13"/>
-      <c r="AL55" s="81"/>
-      <c r="AM55" s="81"/>
+      <c r="AL55" s="50"/>
+      <c r="AM55" s="50"/>
       <c r="AN55" s="12"/>
       <c r="AO55" s="12"/>
       <c r="AP55" s="12"/>
@@ -4483,8 +4484,8 @@
       <c r="A56" s="48"/>
       <c r="B56" s="44"/>
       <c r="C56" s="49"/>
-      <c r="D56" s="84"/>
-      <c r="E56" s="82" t="s">
+      <c r="D56" s="53"/>
+      <c r="E56" s="51" t="s">
         <v>32</v>
       </c>
       <c r="F56" s="12"/>
@@ -4569,12 +4570,12 @@
       <c r="CG56" s="13"/>
     </row>
     <row r="57" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="56">
+      <c r="A57" s="82">
         <v>10</v>
       </c>
-      <c r="B57" s="57"/>
-      <c r="C57" s="60"/>
-      <c r="D57" s="61"/>
+      <c r="B57" s="98"/>
+      <c r="C57" s="76"/>
+      <c r="D57" s="69"/>
       <c r="E57" s="25" t="s">
         <v>4</v>
       </c>
@@ -4600,10 +4601,10 @@
       <c r="CG57" s="17"/>
     </row>
     <row r="58" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="56"/>
-      <c r="B58" s="58"/>
-      <c r="C58" s="62"/>
-      <c r="D58" s="63"/>
+      <c r="A58" s="82"/>
+      <c r="B58" s="70"/>
+      <c r="C58" s="77"/>
+      <c r="D58" s="78"/>
       <c r="E58" s="26" t="s">
         <v>7</v>
       </c>
@@ -4629,10 +4630,10 @@
       <c r="CG58" s="20"/>
     </row>
     <row r="59" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="56"/>
-      <c r="B59" s="58"/>
-      <c r="C59" s="62"/>
-      <c r="D59" s="63"/>
+      <c r="A59" s="82"/>
+      <c r="B59" s="70"/>
+      <c r="C59" s="77"/>
+      <c r="D59" s="78"/>
       <c r="E59" s="26" t="s">
         <v>8</v>
       </c>
@@ -4658,10 +4659,10 @@
       <c r="CG59" s="20"/>
     </row>
     <row r="60" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="56"/>
-      <c r="B60" s="59"/>
-      <c r="C60" s="63"/>
-      <c r="D60" s="63"/>
+      <c r="A60" s="82"/>
+      <c r="B60" s="71"/>
+      <c r="C60" s="78"/>
+      <c r="D60" s="78"/>
       <c r="E60" s="41" t="s">
         <v>9</v>
       </c>
@@ -4747,12 +4748,12 @@
       <c r="CG60" s="20"/>
     </row>
     <row r="61" spans="1:85" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="56">
+      <c r="A61" s="82">
         <v>11</v>
       </c>
-      <c r="B61" s="53"/>
-      <c r="C61" s="53"/>
-      <c r="D61" s="53"/>
+      <c r="B61" s="66"/>
+      <c r="C61" s="66"/>
+      <c r="D61" s="66"/>
       <c r="E61" s="38" t="s">
         <v>4</v>
       </c>
@@ -4778,10 +4779,10 @@
       <c r="CG61" s="11"/>
     </row>
     <row r="62" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="56"/>
-      <c r="B62" s="64"/>
-      <c r="C62" s="54"/>
-      <c r="D62" s="54"/>
+      <c r="A62" s="82"/>
+      <c r="B62" s="80"/>
+      <c r="C62" s="67"/>
+      <c r="D62" s="67"/>
       <c r="E62" s="39" t="s">
         <v>6</v>
       </c>
@@ -4797,10 +4798,10 @@
       <c r="CG62" s="13"/>
     </row>
     <row r="63" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="56"/>
-      <c r="B63" s="64"/>
-      <c r="C63" s="54"/>
-      <c r="D63" s="54"/>
+      <c r="A63" s="82"/>
+      <c r="B63" s="80"/>
+      <c r="C63" s="67"/>
+      <c r="D63" s="67"/>
       <c r="E63" s="40" t="s">
         <v>8</v>
       </c>
@@ -4816,10 +4817,10 @@
       <c r="CG63" s="13"/>
     </row>
     <row r="64" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="56"/>
-      <c r="B64" s="65"/>
-      <c r="C64" s="55"/>
-      <c r="D64" s="55"/>
+      <c r="A64" s="82"/>
+      <c r="B64" s="81"/>
+      <c r="C64" s="68"/>
+      <c r="D64" s="68"/>
       <c r="E64" s="39" t="s">
         <v>9</v>
       </c>
@@ -4905,12 +4906,12 @@
       <c r="CG64" s="13"/>
     </row>
     <row r="65" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="56">
+      <c r="A65" s="82">
         <v>12</v>
       </c>
-      <c r="B65" s="57"/>
-      <c r="C65" s="60"/>
-      <c r="D65" s="61"/>
+      <c r="B65" s="98"/>
+      <c r="C65" s="76"/>
+      <c r="D65" s="69"/>
       <c r="E65" s="25" t="s">
         <v>4</v>
       </c>
@@ -4936,10 +4937,10 @@
       <c r="CG65" s="17"/>
     </row>
     <row r="66" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="56"/>
-      <c r="B66" s="58"/>
-      <c r="C66" s="62"/>
-      <c r="D66" s="63"/>
+      <c r="A66" s="82"/>
+      <c r="B66" s="70"/>
+      <c r="C66" s="77"/>
+      <c r="D66" s="78"/>
       <c r="E66" s="26" t="s">
         <v>6</v>
       </c>
@@ -4965,10 +4966,10 @@
       <c r="CG66" s="20"/>
     </row>
     <row r="67" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="56"/>
-      <c r="B67" s="58"/>
-      <c r="C67" s="62"/>
-      <c r="D67" s="63"/>
+      <c r="A67" s="82"/>
+      <c r="B67" s="70"/>
+      <c r="C67" s="77"/>
+      <c r="D67" s="78"/>
       <c r="E67" s="26" t="s">
         <v>8</v>
       </c>
@@ -4994,10 +4995,10 @@
       <c r="CG67" s="20"/>
     </row>
     <row r="68" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="56"/>
-      <c r="B68" s="59"/>
-      <c r="C68" s="63"/>
-      <c r="D68" s="63"/>
+      <c r="A68" s="82"/>
+      <c r="B68" s="71"/>
+      <c r="C68" s="78"/>
+      <c r="D68" s="78"/>
       <c r="E68" s="41" t="s">
         <v>9</v>
       </c>
@@ -5083,12 +5084,12 @@
       <c r="CG68" s="20"/>
     </row>
     <row r="69" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="56">
+      <c r="A69" s="82">
         <v>13</v>
       </c>
-      <c r="B69" s="70"/>
-      <c r="C69" s="53"/>
-      <c r="D69" s="53"/>
+      <c r="B69" s="79"/>
+      <c r="C69" s="66"/>
+      <c r="D69" s="66"/>
       <c r="E69" s="38" t="s">
         <v>4</v>
       </c>
@@ -5114,10 +5115,10 @@
       <c r="CG69" s="11"/>
     </row>
     <row r="70" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="56"/>
-      <c r="B70" s="64"/>
-      <c r="C70" s="54"/>
-      <c r="D70" s="54"/>
+      <c r="A70" s="82"/>
+      <c r="B70" s="80"/>
+      <c r="C70" s="67"/>
+      <c r="D70" s="67"/>
       <c r="E70" s="39" t="s">
         <v>6</v>
       </c>
@@ -5133,10 +5134,10 @@
       <c r="CG70" s="13"/>
     </row>
     <row r="71" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="56"/>
-      <c r="B71" s="64"/>
-      <c r="C71" s="54"/>
-      <c r="D71" s="54"/>
+      <c r="A71" s="82"/>
+      <c r="B71" s="80"/>
+      <c r="C71" s="67"/>
+      <c r="D71" s="67"/>
       <c r="E71" s="40" t="s">
         <v>8</v>
       </c>
@@ -5152,10 +5153,10 @@
       <c r="CG71" s="13"/>
     </row>
     <row r="72" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="56"/>
-      <c r="B72" s="65"/>
-      <c r="C72" s="55"/>
-      <c r="D72" s="55"/>
+      <c r="A72" s="82"/>
+      <c r="B72" s="81"/>
+      <c r="C72" s="68"/>
+      <c r="D72" s="68"/>
       <c r="E72" s="39" t="s">
         <v>9</v>
       </c>
@@ -5241,12 +5242,12 @@
       <c r="CG72" s="13"/>
     </row>
     <row r="73" spans="1:85" s="16" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="56">
+      <c r="A73" s="82">
         <v>14</v>
       </c>
-      <c r="B73" s="61"/>
-      <c r="C73" s="60"/>
-      <c r="D73" s="61"/>
+      <c r="B73" s="69"/>
+      <c r="C73" s="76"/>
+      <c r="D73" s="69"/>
       <c r="E73" s="25" t="s">
         <v>4</v>
       </c>
@@ -5272,10 +5273,10 @@
       <c r="CG73" s="17"/>
     </row>
     <row r="74" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="56"/>
-      <c r="B74" s="58"/>
-      <c r="C74" s="62"/>
-      <c r="D74" s="63"/>
+      <c r="A74" s="82"/>
+      <c r="B74" s="70"/>
+      <c r="C74" s="77"/>
+      <c r="D74" s="78"/>
       <c r="E74" s="26" t="s">
         <v>6</v>
       </c>
@@ -5301,10 +5302,10 @@
       <c r="CG74" s="20"/>
     </row>
     <row r="75" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="56"/>
-      <c r="B75" s="58"/>
-      <c r="C75" s="62"/>
-      <c r="D75" s="63"/>
+      <c r="A75" s="82"/>
+      <c r="B75" s="70"/>
+      <c r="C75" s="77"/>
+      <c r="D75" s="78"/>
       <c r="E75" s="26" t="s">
         <v>8</v>
       </c>
@@ -5330,10 +5331,10 @@
       <c r="CG75" s="20"/>
     </row>
     <row r="76" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="56"/>
-      <c r="B76" s="59"/>
-      <c r="C76" s="63"/>
-      <c r="D76" s="63"/>
+      <c r="A76" s="82"/>
+      <c r="B76" s="71"/>
+      <c r="C76" s="78"/>
+      <c r="D76" s="78"/>
       <c r="E76" s="41" t="s">
         <v>9</v>
       </c>
@@ -5419,12 +5420,12 @@
       <c r="CG76" s="20"/>
     </row>
     <row r="77" spans="1:85" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="56">
+      <c r="A77" s="82">
         <v>15</v>
       </c>
-      <c r="B77" s="70"/>
-      <c r="C77" s="53"/>
-      <c r="D77" s="53"/>
+      <c r="B77" s="79"/>
+      <c r="C77" s="66"/>
+      <c r="D77" s="66"/>
       <c r="E77" s="38" t="s">
         <v>4</v>
       </c>
@@ -5450,10 +5451,10 @@
       <c r="CG77" s="11"/>
     </row>
     <row r="78" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="56"/>
-      <c r="B78" s="64"/>
-      <c r="C78" s="54"/>
-      <c r="D78" s="54"/>
+      <c r="A78" s="82"/>
+      <c r="B78" s="80"/>
+      <c r="C78" s="67"/>
+      <c r="D78" s="67"/>
       <c r="E78" s="39" t="s">
         <v>6</v>
       </c>
@@ -5469,10 +5470,10 @@
       <c r="CG78" s="13"/>
     </row>
     <row r="79" spans="1:85" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="56"/>
-      <c r="B79" s="64"/>
-      <c r="C79" s="54"/>
-      <c r="D79" s="54"/>
+      <c r="A79" s="82"/>
+      <c r="B79" s="80"/>
+      <c r="C79" s="67"/>
+      <c r="D79" s="67"/>
       <c r="E79" s="40" t="s">
         <v>8</v>
       </c>
@@ -5488,10 +5489,10 @@
       <c r="CG79" s="13"/>
     </row>
     <row r="80" spans="1:85" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="56"/>
-      <c r="B80" s="65"/>
-      <c r="C80" s="55"/>
-      <c r="D80" s="55"/>
+      <c r="A80" s="82"/>
+      <c r="B80" s="81"/>
+      <c r="C80" s="68"/>
+      <c r="D80" s="68"/>
       <c r="E80" s="39" t="s">
         <v>9</v>
       </c>
@@ -5577,12 +5578,12 @@
       <c r="CG80" s="13"/>
     </row>
     <row r="81" spans="1:85" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="56">
+      <c r="A81" s="82">
         <v>16</v>
       </c>
-      <c r="B81" s="61"/>
-      <c r="C81" s="60"/>
-      <c r="D81" s="61"/>
+      <c r="B81" s="69"/>
+      <c r="C81" s="76"/>
+      <c r="D81" s="69"/>
       <c r="E81" s="25" t="s">
         <v>4</v>
       </c>
@@ -5608,10 +5609,10 @@
       <c r="CG81" s="17"/>
     </row>
     <row r="82" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="56"/>
-      <c r="B82" s="58"/>
-      <c r="C82" s="62"/>
-      <c r="D82" s="63"/>
+      <c r="A82" s="82"/>
+      <c r="B82" s="70"/>
+      <c r="C82" s="77"/>
+      <c r="D82" s="78"/>
       <c r="E82" s="26" t="s">
         <v>6</v>
       </c>
@@ -5637,10 +5638,10 @@
       <c r="CG82" s="20"/>
     </row>
     <row r="83" spans="1:85" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="56"/>
-      <c r="B83" s="58"/>
-      <c r="C83" s="62"/>
-      <c r="D83" s="63"/>
+      <c r="A83" s="82"/>
+      <c r="B83" s="70"/>
+      <c r="C83" s="77"/>
+      <c r="D83" s="78"/>
       <c r="E83" s="26" t="s">
         <v>8</v>
       </c>
@@ -5666,10 +5667,10 @@
       <c r="CG83" s="20"/>
     </row>
     <row r="84" spans="1:85" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="56"/>
-      <c r="B84" s="59"/>
-      <c r="C84" s="63"/>
-      <c r="D84" s="63"/>
+      <c r="A84" s="82"/>
+      <c r="B84" s="71"/>
+      <c r="C84" s="78"/>
+      <c r="D84" s="78"/>
       <c r="E84" s="41" t="s">
         <v>9</v>
       </c>
@@ -5755,12 +5756,12 @@
       <c r="CG84" s="20"/>
     </row>
     <row r="85" spans="1:85" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="69"/>
-      <c r="B85" s="71" t="s">
+      <c r="A85" s="83"/>
+      <c r="B85" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="C85" s="73"/>
-      <c r="D85" s="73"/>
+      <c r="C85" s="74"/>
+      <c r="D85" s="74"/>
       <c r="E85" s="29"/>
       <c r="F85" s="30"/>
       <c r="G85" s="31"/>
@@ -5846,10 +5847,10 @@
       <c r="CG85" s="36"/>
     </row>
     <row r="86" spans="1:85" s="14" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="69"/>
-      <c r="B86" s="72"/>
-      <c r="C86" s="74"/>
-      <c r="D86" s="74"/>
+      <c r="A86" s="83"/>
+      <c r="B86" s="73"/>
+      <c r="C86" s="75"/>
+      <c r="D86" s="75"/>
       <c r="E86" s="32"/>
       <c r="F86" s="33"/>
       <c r="G86" s="34"/>
@@ -5934,15 +5935,47 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="C69:D72"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="C85:D86"/>
-    <mergeCell ref="C73:D76"/>
-    <mergeCell ref="B77:B80"/>
-    <mergeCell ref="C77:D80"/>
-    <mergeCell ref="B81:B84"/>
-    <mergeCell ref="C81:D84"/>
+    <mergeCell ref="BJ1:BQ1"/>
+    <mergeCell ref="BR1:BY1"/>
+    <mergeCell ref="BZ1:CG1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:AC1"/>
+    <mergeCell ref="AD1:AK1"/>
+    <mergeCell ref="AL1:AS1"/>
+    <mergeCell ref="AT1:BA1"/>
+    <mergeCell ref="C61:D64"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="C65:D68"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="C51:D54"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="C57:D60"/>
+    <mergeCell ref="C33:D36"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="C39:D42"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="C45:D48"/>
+    <mergeCell ref="C15:D18"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="C21:D24"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:D30"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="BB1:BI1"/>
+    <mergeCell ref="C9:D12"/>
+    <mergeCell ref="F1:M1"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:D6"/>
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="A73:A76"/>
     <mergeCell ref="A77:A80"/>
     <mergeCell ref="A81:A84"/>
@@ -5956,47 +5989,15 @@
     <mergeCell ref="B15:B18"/>
     <mergeCell ref="A33:A36"/>
     <mergeCell ref="B33:B36"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="BB1:BI1"/>
-    <mergeCell ref="C9:D12"/>
-    <mergeCell ref="F1:M1"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:D6"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C15:D18"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="C21:D24"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:D30"/>
-    <mergeCell ref="C33:D36"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="C39:D42"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="C45:D48"/>
-    <mergeCell ref="C61:D64"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="C65:D68"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="C51:D54"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="C57:D60"/>
-    <mergeCell ref="BJ1:BQ1"/>
-    <mergeCell ref="BR1:BY1"/>
-    <mergeCell ref="BZ1:CG1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:AC1"/>
-    <mergeCell ref="AD1:AK1"/>
-    <mergeCell ref="AL1:AS1"/>
-    <mergeCell ref="AT1:BA1"/>
+    <mergeCell ref="C69:D72"/>
+    <mergeCell ref="B73:B76"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="C85:D86"/>
+    <mergeCell ref="C73:D76"/>
+    <mergeCell ref="B77:B80"/>
+    <mergeCell ref="C77:D80"/>
+    <mergeCell ref="B81:B84"/>
+    <mergeCell ref="C81:D84"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>